<commit_message>
played with data by seperating indiviual harvest dates, also by speerating data by year and plotting individually
</commit_message>
<xml_diff>
--- a/data/ORG Harvest DATA for R.xlsx
+++ b/data/ORG Harvest DATA for R.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharyhirsch-santagata/Desktop/2025 STAT/CRSS 8030/org_harvest/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10F18E5-580D-584A-9536-DB527FFE1B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FFA152-5BC5-5443-BF41-96B48D9C6465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="580" windowWidth="27640" windowHeight="16940" xr2:uid="{522299A1-AB87-F342-A22C-ACEE8B2E13C2}"/>
+    <workbookView xWindow="4540" yWindow="2380" windowWidth="27640" windowHeight="16940" xr2:uid="{522299A1-AB87-F342-A22C-ACEE8B2E13C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Harvest Totals for R" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -521,10 +521,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C169B2FA-7165-674F-99C1-BC7586B9A24F}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="70" workbookViewId="0">
-      <selection activeCell="R238" sqref="R238"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="83" workbookViewId="0">
+      <selection activeCell="N216" sqref="N216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3872,22 +3873,22 @@
       <c r="G82" t="s">
         <v>8</v>
       </c>
-      <c r="H82">
+      <c r="H82" s="4">
         <v>1715.5336727499998</v>
       </c>
-      <c r="I82">
+      <c r="I82" s="4">
         <v>2028.1018388520322</v>
       </c>
-      <c r="J82">
+      <c r="J82" s="4">
         <v>872.07645000000002</v>
       </c>
-      <c r="K82">
+      <c r="K82" s="4">
         <v>1744.1529</v>
       </c>
-      <c r="L82">
+      <c r="L82" s="4">
         <v>2587.6101227499998</v>
       </c>
-      <c r="M82">
+      <c r="M82" s="4">
         <v>1779.2495703247066</v>
       </c>
     </row>
@@ -3913,22 +3914,22 @@
       <c r="G83" t="s">
         <v>8</v>
       </c>
-      <c r="H83">
+      <c r="H83" s="4">
         <v>2816.7953649999999</v>
       </c>
-      <c r="I83">
+      <c r="I83" s="4">
         <v>2564.860692328501</v>
       </c>
-      <c r="J83">
+      <c r="J83" s="4">
         <v>1220.9070325</v>
       </c>
-      <c r="K83">
+      <c r="K83" s="4">
         <v>2441.814065</v>
       </c>
-      <c r="L83">
+      <c r="L83" s="4">
         <v>4037.7023975000002</v>
       </c>
-      <c r="M83">
+      <c r="M83" s="4">
         <v>1835.8047041479972</v>
       </c>
     </row>
@@ -3954,22 +3955,22 @@
       <c r="G84" t="s">
         <v>8</v>
       </c>
-      <c r="H84">
+      <c r="H84" s="4">
         <v>3593.1401150000002</v>
       </c>
-      <c r="I84">
+      <c r="I84" s="4">
         <v>2601.5906431166954</v>
       </c>
-      <c r="J84">
+      <c r="J84" s="4">
         <v>3403.9909377499998</v>
       </c>
-      <c r="K84">
+      <c r="K84" s="4">
         <v>3909.4727424983525</v>
       </c>
-      <c r="L84">
+      <c r="L84" s="4">
         <v>6997.13105275</v>
       </c>
-      <c r="M84">
+      <c r="M84" s="4">
         <v>2233.688258746718</v>
       </c>
     </row>
@@ -3995,22 +3996,22 @@
       <c r="G85" t="s">
         <v>8</v>
       </c>
-      <c r="H85">
+      <c r="H85" s="4">
         <v>4481.1847099999995</v>
       </c>
-      <c r="I85">
+      <c r="I85" s="4">
         <v>3147.4344311892773</v>
       </c>
-      <c r="J85">
+      <c r="J85" s="4">
         <v>4410.6780402499999</v>
       </c>
-      <c r="K85">
+      <c r="K85" s="4">
         <v>3510.8292135127349</v>
       </c>
-      <c r="L85">
+      <c r="L85" s="4">
         <v>8891.8627502500003</v>
       </c>
-      <c r="M85">
+      <c r="M85" s="4">
         <v>2369.6821601676843</v>
       </c>
     </row>
@@ -4036,22 +4037,22 @@
       <c r="G86" t="s">
         <v>8</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="4">
         <v>5270.6433900000002</v>
       </c>
-      <c r="I86">
+      <c r="I86" s="4">
         <v>3549.4674633624586</v>
       </c>
-      <c r="J86">
+      <c r="J86" s="4">
         <v>4840.8149952499998</v>
       </c>
-      <c r="K86">
+      <c r="K86" s="4">
         <v>3674.7781228243612</v>
       </c>
-      <c r="L86">
+      <c r="L86" s="4">
         <v>10111.45838525</v>
       </c>
-      <c r="M86">
+      <c r="M86" s="4">
         <v>1548.2517026310511</v>
       </c>
     </row>
@@ -4077,22 +4078,22 @@
       <c r="G87" t="s">
         <v>9</v>
       </c>
-      <c r="H87">
+      <c r="H87" s="4">
         <v>1233.3652649999999</v>
       </c>
-      <c r="I87">
+      <c r="I87" s="4">
         <v>1693.0370089025153</v>
       </c>
-      <c r="J87">
+      <c r="J87" s="4">
         <v>0</v>
       </c>
-      <c r="K87">
+      <c r="K87" s="4">
         <v>0</v>
       </c>
-      <c r="L87">
+      <c r="L87" s="4">
         <v>1233.3652649999999</v>
       </c>
-      <c r="M87">
+      <c r="M87" s="4">
         <v>1693.0370089025153</v>
       </c>
     </row>
@@ -4118,22 +4119,22 @@
       <c r="G88" t="s">
         <v>9</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="4">
         <v>1420.2387899999999</v>
       </c>
-      <c r="I88">
+      <c r="I88" s="4">
         <v>1644.4870200000003</v>
       </c>
-      <c r="J88">
+      <c r="J88" s="4">
         <v>426.36670100000003</v>
       </c>
-      <c r="K88">
+      <c r="K88" s="4">
         <v>295.86396415386923</v>
       </c>
-      <c r="L88">
+      <c r="L88" s="4">
         <v>1846.605491</v>
       </c>
-      <c r="M88">
+      <c r="M88" s="4">
         <v>1725.3544130697655</v>
       </c>
     </row>
@@ -4159,22 +4160,22 @@
       <c r="G89" t="s">
         <v>9</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="4">
         <v>2803.102875</v>
       </c>
-      <c r="I89">
+      <c r="I89" s="4">
         <v>1179.525794351983</v>
       </c>
-      <c r="J89">
+      <c r="J89" s="4">
         <v>2129.3746424999999</v>
       </c>
-      <c r="K89">
+      <c r="K89" s="4">
         <v>768.35189758146271</v>
       </c>
-      <c r="L89">
+      <c r="L89" s="4">
         <v>4932.4775174999995</v>
       </c>
-      <c r="M89">
+      <c r="M89" s="4">
         <v>1614.1202918148203</v>
       </c>
     </row>
@@ -4200,22 +4201,22 @@
       <c r="G90" t="s">
         <v>9</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="4">
         <v>4182.8524024999997</v>
       </c>
-      <c r="I90">
+      <c r="I90" s="4">
         <v>3202.9114292698005</v>
       </c>
-      <c r="J90">
+      <c r="J90" s="4">
         <v>4815.2717600000005</v>
       </c>
-      <c r="K90">
+      <c r="K90" s="4">
         <v>1680.2800580976966</v>
       </c>
-      <c r="L90">
+      <c r="L90" s="4">
         <v>8998.1241625000002</v>
       </c>
-      <c r="M90">
+      <c r="M90" s="4">
         <v>1799.6715169797014</v>
       </c>
     </row>
@@ -4241,22 +4242,22 @@
       <c r="G91" t="s">
         <v>9</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="4">
         <v>4958.3775450000003</v>
       </c>
-      <c r="I91">
+      <c r="I91" s="4">
         <v>3966.964982178541</v>
       </c>
-      <c r="J91">
+      <c r="J91" s="4">
         <v>5406.3822250000003</v>
       </c>
-      <c r="K91">
+      <c r="K91" s="4">
         <v>2075.8498606994744</v>
       </c>
-      <c r="L91">
+      <c r="L91" s="4">
         <v>10364.759770000001</v>
       </c>
-      <c r="M91">
+      <c r="M91" s="4">
         <v>2166.994414960503</v>
       </c>
     </row>
@@ -4282,22 +4283,22 @@
       <c r="G92" t="s">
         <v>8</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="4">
         <v>5369.0639950000004</v>
       </c>
-      <c r="I92">
+      <c r="I92" s="4">
         <v>2327.2351618580656</v>
       </c>
-      <c r="J92">
+      <c r="J92" s="4">
         <v>0</v>
       </c>
-      <c r="K92">
+      <c r="K92" s="4">
         <v>0</v>
       </c>
-      <c r="L92">
+      <c r="L92" s="4">
         <v>5369.0639950000004</v>
       </c>
-      <c r="M92">
+      <c r="M92" s="4">
         <v>2327.2351618580656</v>
       </c>
     </row>
@@ -4323,22 +4324,22 @@
       <c r="G93" t="s">
         <v>8</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="4">
         <v>7206.3919325000006</v>
       </c>
-      <c r="I93">
+      <c r="I93" s="4">
         <v>1329.6142274247748</v>
       </c>
-      <c r="J93">
+      <c r="J93" s="4">
         <v>677.60455849999994</v>
       </c>
-      <c r="K93">
+      <c r="K93" s="4">
         <v>979.6714528551413</v>
       </c>
-      <c r="L93">
+      <c r="L93" s="4">
         <v>7883.9964910000008</v>
       </c>
-      <c r="M93">
+      <c r="M93" s="4">
         <v>1906.6538370373485</v>
       </c>
     </row>
@@ -4364,22 +4365,22 @@
       <c r="G94" t="s">
         <v>8</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="4">
         <v>7206.3919325000006</v>
       </c>
-      <c r="I94">
+      <c r="I94" s="4">
         <v>1329.6142274247748</v>
       </c>
-      <c r="J94">
+      <c r="J94" s="4">
         <v>2377.76518025</v>
       </c>
-      <c r="K94">
+      <c r="K94" s="4">
         <v>1558.4119707867058</v>
       </c>
-      <c r="L94">
+      <c r="L94" s="4">
         <v>9584.1571127499992</v>
       </c>
-      <c r="M94">
+      <c r="M94" s="4">
         <v>707.14647026719945</v>
       </c>
     </row>
@@ -4405,22 +4406,22 @@
       <c r="G95" t="s">
         <v>8</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="4">
         <v>7677.5016599999999</v>
       </c>
-      <c r="I95">
+      <c r="I95" s="4">
         <v>1370.3500382931193</v>
       </c>
-      <c r="J95">
+      <c r="J95" s="4">
         <v>3119.6390252499996</v>
       </c>
-      <c r="K95">
+      <c r="K95" s="4">
         <v>2618.6716206579458</v>
       </c>
-      <c r="L95">
+      <c r="L95" s="4">
         <v>10797.14068525</v>
       </c>
-      <c r="M95">
+      <c r="M95" s="4">
         <v>1407.6712129906671</v>
       </c>
     </row>
@@ -4446,22 +4447,22 @@
       <c r="G96" t="s">
         <v>8</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="4">
         <v>7677.5016599999999</v>
       </c>
-      <c r="I96">
+      <c r="I96" s="4">
         <v>1370.3500382931193</v>
       </c>
-      <c r="J96">
+      <c r="J96" s="4">
         <v>3686.8551352499999</v>
       </c>
-      <c r="K96">
+      <c r="K96" s="4">
         <v>2818.0103381897497</v>
       </c>
-      <c r="L96">
+      <c r="L96" s="4">
         <v>11364.356795250002</v>
       </c>
-      <c r="M96">
+      <c r="M96" s="4">
         <v>1761.9504105412004</v>
       </c>
     </row>
@@ -4487,22 +4488,22 @@
       <c r="G97" t="s">
         <v>9</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="4">
         <v>1761.9242077499998</v>
       </c>
-      <c r="I97">
+      <c r="I97" s="4">
         <v>1303.7430378514973</v>
       </c>
-      <c r="J97">
+      <c r="J97" s="4">
         <v>0</v>
       </c>
-      <c r="K97">
+      <c r="K97" s="4">
         <v>0</v>
       </c>
-      <c r="L97">
+      <c r="L97" s="4">
         <v>1761.9242077499998</v>
       </c>
-      <c r="M97">
+      <c r="M97" s="4">
         <v>1303.7430378514973</v>
       </c>
     </row>
@@ -4528,22 +4529,22 @@
       <c r="G98" t="s">
         <v>9</v>
       </c>
-      <c r="H98">
+      <c r="H98" s="4">
         <v>2135.6712575000001</v>
       </c>
-      <c r="I98">
+      <c r="I98" s="4">
         <v>999.56013055457265</v>
       </c>
-      <c r="J98">
+      <c r="J98" s="4">
         <v>2437.05062</v>
       </c>
-      <c r="K98">
+      <c r="K98" s="4">
         <v>2093.0793174797118</v>
       </c>
-      <c r="L98">
+      <c r="L98" s="4">
         <v>4572.7218775000001</v>
       </c>
-      <c r="M98">
+      <c r="M98" s="4">
         <v>1913.6941824975409</v>
       </c>
     </row>
@@ -4569,22 +4570,22 @@
       <c r="G99" t="s">
         <v>9</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="4">
         <v>3266.8057125</v>
       </c>
-      <c r="I99">
+      <c r="I99" s="4">
         <v>1425.7030526307274</v>
       </c>
-      <c r="J99">
+      <c r="J99" s="4">
         <v>5545.1970425</v>
       </c>
-      <c r="K99">
+      <c r="K99" s="4">
         <v>3111.88820430637</v>
       </c>
-      <c r="L99">
+      <c r="L99" s="4">
         <v>8812.0027549999995</v>
       </c>
-      <c r="M99">
+      <c r="M99" s="4">
         <v>2226.4022154306399</v>
       </c>
     </row>
@@ -4610,22 +4611,22 @@
       <c r="G100" t="s">
         <v>9</v>
       </c>
-      <c r="H100">
+      <c r="H100" s="4">
         <v>4510.4307024999998</v>
       </c>
-      <c r="I100">
+      <c r="I100" s="4">
         <v>2328.9670562363526</v>
       </c>
-      <c r="J100">
+      <c r="J100" s="4">
         <v>6473.3355525000006</v>
       </c>
-      <c r="K100">
+      <c r="K100" s="4">
         <v>2836.396990693469</v>
       </c>
-      <c r="L100">
+      <c r="L100" s="4">
         <v>10983.766254999999</v>
       </c>
-      <c r="M100">
+      <c r="M100" s="4">
         <v>795.57587223776795</v>
       </c>
     </row>
@@ -4651,22 +4652,22 @@
       <c r="G101" t="s">
         <v>9</v>
       </c>
-      <c r="H101">
+      <c r="H101" s="4">
         <v>4709.7624624999999</v>
       </c>
-      <c r="I101">
+      <c r="I101" s="4">
         <v>2685.4770844224768</v>
       </c>
-      <c r="J101">
+      <c r="J101" s="4">
         <v>6772.3331925000002</v>
       </c>
-      <c r="K101">
+      <c r="K101" s="4">
         <v>2303.8022044090371</v>
       </c>
-      <c r="L101">
+      <c r="L101" s="4">
         <v>11482.095655000001</v>
       </c>
-      <c r="M101">
+      <c r="M101" s="4">
         <v>734.47341930930429</v>
       </c>
     </row>
@@ -4692,22 +4693,22 @@
       <c r="G102" t="s">
         <v>8</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="4">
         <v>1490.0049075000002</v>
       </c>
-      <c r="I102">
+      <c r="I102" s="4">
         <v>1814.9318213534364</v>
       </c>
-      <c r="J102">
+      <c r="J102" s="4">
         <v>0</v>
       </c>
-      <c r="K102">
+      <c r="K102" s="4">
         <v>0</v>
       </c>
-      <c r="L102">
+      <c r="L102" s="4">
         <v>1490.0049075000002</v>
       </c>
-      <c r="M102">
+      <c r="M102" s="4">
         <v>1814.9318213534364</v>
       </c>
     </row>
@@ -4733,22 +4734,22 @@
       <c r="G103" t="s">
         <v>8</v>
       </c>
-      <c r="H103">
+      <c r="H103" s="4">
         <v>4682.591555</v>
       </c>
-      <c r="I103">
+      <c r="I103" s="4">
         <v>1044.3093670896651</v>
       </c>
-      <c r="J103">
+      <c r="J103" s="4">
         <v>1619.5705499999999</v>
       </c>
-      <c r="K103">
+      <c r="K103" s="4">
         <v>2255.7319414394824</v>
       </c>
-      <c r="L103">
+      <c r="L103" s="4">
         <v>6302.1621050000003</v>
       </c>
-      <c r="M103">
+      <c r="M103" s="4">
         <v>2235.3804666268261</v>
       </c>
     </row>
@@ -4774,22 +4775,22 @@
       <c r="G104" t="s">
         <v>8</v>
       </c>
-      <c r="H104">
+      <c r="H104" s="4">
         <v>7656.8312624999999</v>
       </c>
-      <c r="I104">
+      <c r="I104" s="4">
         <v>4050.5598321883449</v>
       </c>
-      <c r="J104">
+      <c r="J104" s="4">
         <v>2688.09369625</v>
       </c>
-      <c r="K104">
+      <c r="K104" s="4">
         <v>3079.121691241518</v>
       </c>
-      <c r="L104">
+      <c r="L104" s="4">
         <v>10344.92495875</v>
       </c>
-      <c r="M104">
+      <c r="M104" s="4">
         <v>2114.1288969438874</v>
       </c>
     </row>
@@ -4815,22 +4816,22 @@
       <c r="G105" t="s">
         <v>8</v>
       </c>
-      <c r="H105">
+      <c r="H105" s="4">
         <v>8149.3905099999993</v>
       </c>
-      <c r="I105">
+      <c r="I105" s="4">
         <v>4173.9549956966148</v>
       </c>
-      <c r="J105">
+      <c r="J105" s="4">
         <v>3736.6836700000003</v>
       </c>
-      <c r="K105">
+      <c r="K105" s="4">
         <v>3823.0534117086272</v>
       </c>
-      <c r="L105">
+      <c r="L105" s="4">
         <v>11886.07418</v>
       </c>
-      <c r="M105">
+      <c r="M105" s="4">
         <v>1901.133468285545</v>
       </c>
     </row>
@@ -4856,22 +4857,22 @@
       <c r="G106" t="s">
         <v>8</v>
       </c>
-      <c r="H106">
+      <c r="H106" s="4">
         <v>8149.3905099999993</v>
       </c>
-      <c r="I106">
+      <c r="I106" s="4">
         <v>4173.9549956966148</v>
       </c>
-      <c r="J106">
+      <c r="J106" s="4">
         <v>4085.5142500000002</v>
       </c>
-      <c r="K106">
+      <c r="K106" s="4">
         <v>4112.3057720711195</v>
       </c>
-      <c r="L106">
+      <c r="L106" s="4">
         <v>12234.904760000001</v>
       </c>
-      <c r="M106">
+      <c r="M106" s="4">
         <v>1326.3637711781769</v>
       </c>
     </row>
@@ -4897,22 +4898,22 @@
       <c r="G107" t="s">
         <v>9</v>
       </c>
-      <c r="H107">
+      <c r="H107" s="4">
         <v>872.07645000000002</v>
       </c>
-      <c r="I107">
+      <c r="I107" s="4">
         <v>1007.808841397431</v>
       </c>
-      <c r="J107">
+      <c r="J107" s="4">
         <v>0</v>
       </c>
-      <c r="K107">
+      <c r="K107" s="4">
         <v>0</v>
       </c>
-      <c r="L107">
+      <c r="L107" s="4">
         <v>872.07645000000002</v>
       </c>
-      <c r="M107">
+      <c r="M107" s="4">
         <v>1007.808841397431</v>
       </c>
     </row>
@@ -4938,22 +4939,22 @@
       <c r="G108" t="s">
         <v>9</v>
       </c>
-      <c r="H108">
+      <c r="H108" s="4">
         <v>2496.0440252500002</v>
       </c>
-      <c r="I108">
+      <c r="I108" s="4">
         <v>1622.4067894870127</v>
       </c>
-      <c r="J108">
+      <c r="J108" s="4">
         <v>298.99763999999999</v>
       </c>
-      <c r="K108">
+      <c r="K108" s="4">
         <v>597.99527999999998</v>
       </c>
-      <c r="L108">
+      <c r="L108" s="4">
         <v>2795.0416652499998</v>
       </c>
-      <c r="M108">
+      <c r="M108" s="4">
         <v>1533.1555268899788</v>
       </c>
     </row>
@@ -4979,22 +4980,22 @@
       <c r="G109" t="s">
         <v>9</v>
       </c>
-      <c r="H109">
+      <c r="H109" s="4">
         <v>3886.2364875000003</v>
       </c>
-      <c r="I109">
+      <c r="I109" s="4">
         <v>2116.71897155121</v>
       </c>
-      <c r="J109">
+      <c r="J109" s="4">
         <v>1097.7903550000001</v>
       </c>
-      <c r="K109">
+      <c r="K109" s="4">
         <v>1290.4631145797789</v>
       </c>
-      <c r="L109">
+      <c r="L109" s="4">
         <v>4984.0268424999995</v>
       </c>
-      <c r="M109">
+      <c r="M109" s="4">
         <v>1787.7873316029641</v>
       </c>
     </row>
@@ -5020,22 +5021,22 @@
       <c r="G110" t="s">
         <v>9</v>
       </c>
-      <c r="H110">
+      <c r="H110" s="4">
         <v>7056.4908750000013</v>
       </c>
-      <c r="I110">
+      <c r="I110" s="4">
         <v>4033.0960533804296</v>
       </c>
-      <c r="J110">
+      <c r="J110" s="4">
         <v>1387.9939475000001</v>
       </c>
-      <c r="K110">
+      <c r="K110" s="4">
         <v>1619.4452015351155</v>
       </c>
-      <c r="L110">
+      <c r="L110" s="4">
         <v>8444.4848225000005</v>
       </c>
-      <c r="M110">
+      <c r="M110" s="4">
         <v>3024.6615108450978</v>
       </c>
     </row>
@@ -5061,22 +5062,22 @@
       <c r="G111" t="s">
         <v>9</v>
       </c>
-      <c r="H111">
+      <c r="H111" s="4">
         <v>8383.6593274999996</v>
       </c>
-      <c r="I111">
+      <c r="I111" s="4">
         <v>5129.4538652826823</v>
       </c>
-      <c r="J111">
+      <c r="J111" s="4">
         <v>1961.0727577500002</v>
       </c>
-      <c r="K111">
+      <c r="K111" s="4">
         <v>1762.5155290467367</v>
       </c>
-      <c r="L111">
+      <c r="L111" s="4">
         <v>10344.732085250002</v>
       </c>
-      <c r="M111">
+      <c r="M111" s="4">
         <v>3564.5160717016452</v>
       </c>
     </row>
@@ -5102,22 +5103,22 @@
       <c r="G112" t="s">
         <v>8</v>
       </c>
-      <c r="H112">
+      <c r="H112" s="4">
         <v>2923.0953525000004</v>
       </c>
-      <c r="I112">
+      <c r="I112" s="4">
         <v>2093.2195644644921</v>
       </c>
-      <c r="J112">
+      <c r="J112" s="4">
         <v>0</v>
       </c>
-      <c r="K112">
+      <c r="K112" s="4">
         <v>0</v>
       </c>
-      <c r="L112">
+      <c r="L112" s="4">
         <v>2923.0953525000004</v>
       </c>
-      <c r="M112">
+      <c r="M112" s="4">
         <v>2093.2195644644921</v>
       </c>
     </row>
@@ -5143,22 +5144,22 @@
       <c r="G113" t="s">
         <v>8</v>
       </c>
-      <c r="H113">
+      <c r="H113" s="4">
         <v>5834.0796099999998</v>
       </c>
-      <c r="I113">
+      <c r="I113" s="4">
         <v>3582.2231456881923</v>
       </c>
-      <c r="J113">
+      <c r="J113" s="4">
         <v>946.82586025000001</v>
       </c>
-      <c r="K113">
+      <c r="K113" s="4">
         <v>1465.9131028564707</v>
       </c>
-      <c r="L113">
+      <c r="L113" s="4">
         <v>6780.9054702500007</v>
       </c>
-      <c r="M113">
+      <c r="M113" s="4">
         <v>3877.9236209145911</v>
       </c>
     </row>
@@ -5184,22 +5185,22 @@
       <c r="G114" t="s">
         <v>8</v>
       </c>
-      <c r="H114">
+      <c r="H114" s="4">
         <v>8186.6417975000004</v>
       </c>
-      <c r="I114">
+      <c r="I114" s="4">
         <v>2059.4535598127782</v>
       </c>
-      <c r="J114">
+      <c r="J114" s="4">
         <v>1263.4115977500001</v>
       </c>
-      <c r="K114">
+      <c r="K114" s="4">
         <v>1323.0532263958416</v>
       </c>
-      <c r="L114">
+      <c r="L114" s="4">
         <v>9450.0533952500009</v>
       </c>
-      <c r="M114">
+      <c r="M114" s="4">
         <v>1290.0916552616457</v>
       </c>
     </row>
@@ -5225,22 +5226,22 @@
       <c r="G115" t="s">
         <v>8</v>
       </c>
-      <c r="H115">
+      <c r="H115" s="4">
         <v>9603.4863924999991</v>
       </c>
-      <c r="I115">
+      <c r="I115" s="4">
         <v>2701.3214129937528</v>
       </c>
-      <c r="J115">
+      <c r="J115" s="4">
         <v>2766.34530025</v>
       </c>
-      <c r="K115">
+      <c r="K115" s="4">
         <v>3433.3623451517115</v>
       </c>
-      <c r="L115">
+      <c r="L115" s="4">
         <v>12369.831692750002</v>
       </c>
-      <c r="M115">
+      <c r="M115" s="4">
         <v>1324.9415839092101</v>
       </c>
     </row>
@@ -5266,22 +5267,22 @@
       <c r="G116" t="s">
         <v>8</v>
       </c>
-      <c r="H116">
+      <c r="H116" s="4">
         <v>10012.641042499999</v>
       </c>
-      <c r="I116">
+      <c r="I116" s="4">
         <v>2959.4780815180538</v>
       </c>
-      <c r="J116">
+      <c r="J116" s="4">
         <v>3030.16674775</v>
       </c>
-      <c r="K116">
+      <c r="K116" s="4">
         <v>3417.4951986410624</v>
       </c>
-      <c r="L116">
+      <c r="L116" s="4">
         <v>13042.807790250001</v>
       </c>
-      <c r="M116">
+      <c r="M116" s="4">
         <v>1110.0737659300057</v>
       </c>
     </row>
@@ -5307,22 +5308,22 @@
       <c r="G117" t="s">
         <v>9</v>
       </c>
-      <c r="H117">
+      <c r="H117" s="4">
         <v>1335.7696450000001</v>
       </c>
-      <c r="I117">
+      <c r="I117" s="4">
         <v>1568.6509027416212</v>
       </c>
-      <c r="J117">
+      <c r="J117" s="4">
         <v>0</v>
       </c>
-      <c r="K117">
+      <c r="K117" s="4">
         <v>0</v>
       </c>
-      <c r="L117">
+      <c r="L117" s="4">
         <v>1335.7696450000001</v>
       </c>
-      <c r="M117">
+      <c r="M117" s="4">
         <v>1568.6509027416212</v>
       </c>
     </row>
@@ -5348,22 +5349,22 @@
       <c r="G118" t="s">
         <v>9</v>
       </c>
-      <c r="H118">
+      <c r="H118" s="4">
         <v>4532.0679499999997</v>
       </c>
-      <c r="I118">
+      <c r="I118" s="4">
         <v>1267.0223715413076</v>
       </c>
-      <c r="J118">
+      <c r="J118" s="4">
         <v>472.10153750000001</v>
       </c>
-      <c r="K118">
+      <c r="K118" s="4">
         <v>944.20307500000001</v>
       </c>
-      <c r="L118">
+      <c r="L118" s="4">
         <v>5004.1694875000003</v>
       </c>
-      <c r="M118">
+      <c r="M118" s="4">
         <v>771.42170741777056</v>
       </c>
     </row>
@@ -5389,22 +5390,22 @@
       <c r="G119" t="s">
         <v>9</v>
       </c>
-      <c r="H119">
+      <c r="H119" s="4">
         <v>6849.6378999999997</v>
       </c>
-      <c r="I119">
+      <c r="I119" s="4">
         <v>3639.6540831954562</v>
       </c>
-      <c r="J119">
+      <c r="J119" s="4">
         <v>1231.0955475000001</v>
       </c>
-      <c r="K119">
+      <c r="K119" s="4">
         <v>1735.9114259868313</v>
       </c>
-      <c r="L119">
+      <c r="L119" s="4">
         <v>8080.7334475000007</v>
       </c>
-      <c r="M119">
+      <c r="M119" s="4">
         <v>2376.407905734965</v>
       </c>
     </row>
@@ -5430,22 +5431,22 @@
       <c r="G120" t="s">
         <v>9</v>
       </c>
-      <c r="H120">
+      <c r="H120" s="4">
         <v>9045.4440875</v>
       </c>
-      <c r="I120">
+      <c r="I120" s="4">
         <v>4324.765673484384</v>
       </c>
-      <c r="J120">
+      <c r="J120" s="4">
         <v>1821.2224700000002</v>
       </c>
-      <c r="K120">
+      <c r="K120" s="4">
         <v>2874.7041041069797</v>
       </c>
-      <c r="L120">
+      <c r="L120" s="4">
         <v>10866.666557500001</v>
       </c>
-      <c r="M120">
+      <c r="M120" s="4">
         <v>2139.9045300651596</v>
       </c>
     </row>
@@ -5471,22 +5472,22 @@
       <c r="G121" t="s">
         <v>9</v>
       </c>
-      <c r="H121">
+      <c r="H121" s="4">
         <v>9704.9977099999996</v>
       </c>
-      <c r="I121">
+      <c r="I121" s="4">
         <v>4659.8280128065635</v>
       </c>
-      <c r="J121">
+      <c r="J121" s="4">
         <v>2491.2434975000001</v>
       </c>
-      <c r="K121">
+      <c r="K121" s="4">
         <v>3137.0036847815372</v>
       </c>
-      <c r="L121">
+      <c r="L121" s="4">
         <v>12196.241207499999</v>
       </c>
-      <c r="M121">
+      <c r="M121" s="4">
         <v>2496.1927361838361</v>
       </c>
     </row>
@@ -5512,22 +5513,22 @@
       <c r="G122" t="s">
         <v>8</v>
       </c>
-      <c r="H122">
+      <c r="H122" s="4">
         <v>2758.2532325000002</v>
       </c>
-      <c r="I122">
+      <c r="I122" s="4">
         <v>1958.8571712983075</v>
       </c>
-      <c r="J122">
+      <c r="J122" s="4">
         <v>174.41529025</v>
       </c>
-      <c r="K122">
+      <c r="K122" s="4">
         <v>348.8305805</v>
       </c>
-      <c r="L122">
+      <c r="L122" s="4">
         <v>2932.6685227500002</v>
       </c>
-      <c r="M122">
+      <c r="M122" s="4">
         <v>2005.0498792921042</v>
       </c>
     </row>
@@ -5553,22 +5554,22 @@
       <c r="G123" t="s">
         <v>8</v>
       </c>
-      <c r="H123">
+      <c r="H123" s="4">
         <v>4873.0386249999992</v>
       </c>
-      <c r="I123">
+      <c r="I123" s="4">
         <v>3264.3354937865238</v>
       </c>
-      <c r="J123">
+      <c r="J123" s="4">
         <v>1793.9858399999998</v>
       </c>
-      <c r="K123">
+      <c r="K123" s="4">
         <v>1464.7833045927546</v>
       </c>
-      <c r="L123">
+      <c r="L123" s="4">
         <v>6667.0244650000004</v>
       </c>
-      <c r="M123">
+      <c r="M123" s="4">
         <v>2017.6991438758159</v>
       </c>
     </row>
@@ -5594,22 +5595,22 @@
       <c r="G124" t="s">
         <v>8</v>
       </c>
-      <c r="H124">
+      <c r="H124" s="4">
         <v>6433.4325624999992</v>
       </c>
-      <c r="I124">
+      <c r="I124" s="4">
         <v>5005.9761747023995</v>
       </c>
-      <c r="J124">
+      <c r="J124" s="4">
         <v>3523.1888600000002</v>
       </c>
-      <c r="K124">
+      <c r="K124" s="4">
         <v>3112.5288945552952</v>
       </c>
-      <c r="L124">
+      <c r="L124" s="4">
         <v>9956.6214225000003</v>
       </c>
-      <c r="M124">
+      <c r="M124" s="4">
         <v>2135.8284210805209</v>
       </c>
     </row>
@@ -5635,22 +5636,22 @@
       <c r="G125" t="s">
         <v>8</v>
       </c>
-      <c r="H125">
+      <c r="H125" s="4">
         <v>6433.4325624999992</v>
       </c>
-      <c r="I125">
+      <c r="I125" s="4">
         <v>5005.9761747023995</v>
       </c>
-      <c r="J125">
+      <c r="J125" s="4">
         <v>3847.1029724999999</v>
       </c>
-      <c r="K125">
+      <c r="K125" s="4">
         <v>3418.9513058405428</v>
       </c>
-      <c r="L125">
+      <c r="L125" s="4">
         <v>10280.535534999999</v>
       </c>
-      <c r="M125">
+      <c r="M125" s="4">
         <v>1788.6901991817358</v>
       </c>
     </row>
@@ -5676,22 +5677,22 @@
       <c r="G126" t="s">
         <v>8</v>
       </c>
-      <c r="H126">
+      <c r="H126" s="4">
         <v>6797.8359374999991</v>
       </c>
-      <c r="I126">
+      <c r="I126" s="4">
         <v>5616.2587096074913</v>
       </c>
-      <c r="J126">
+      <c r="J126" s="4">
         <v>4783.9622524999995</v>
       </c>
-      <c r="K126">
+      <c r="K126" s="4">
         <v>4471.2858408465327</v>
       </c>
-      <c r="L126">
+      <c r="L126" s="4">
         <v>11581.798190000001</v>
       </c>
-      <c r="M126">
+      <c r="M126" s="4">
         <v>1722.2891534392568</v>
       </c>
     </row>
@@ -5717,22 +5718,22 @@
       <c r="G127" t="s">
         <v>9</v>
       </c>
-      <c r="H127">
+      <c r="H127" s="4">
         <v>350.50563725000001</v>
       </c>
-      <c r="I127">
+      <c r="I127" s="4">
         <v>408.5018498692811</v>
       </c>
-      <c r="J127">
+      <c r="J127" s="4">
         <v>0</v>
       </c>
-      <c r="K127">
+      <c r="K127" s="4">
         <v>0</v>
       </c>
-      <c r="L127">
+      <c r="L127" s="4">
         <v>350.50563725000001</v>
       </c>
-      <c r="M127">
+      <c r="M127" s="4">
         <v>408.5018498692811</v>
       </c>
     </row>
@@ -5758,22 +5759,22 @@
       <c r="G128" t="s">
         <v>9</v>
       </c>
-      <c r="H128">
+      <c r="H128" s="4">
         <v>1348.82998</v>
       </c>
-      <c r="I128">
+      <c r="I128" s="4">
         <v>716.79984599015631</v>
       </c>
-      <c r="J128">
+      <c r="J128" s="4">
         <v>718.59937050000008</v>
       </c>
-      <c r="K128">
+      <c r="K128" s="4">
         <v>612.54539462672528</v>
       </c>
-      <c r="L128">
+      <c r="L128" s="4">
         <v>2067.4293505000001</v>
       </c>
-      <c r="M128">
+      <c r="M128" s="4">
         <v>185.75880120016359</v>
       </c>
     </row>
@@ -5799,22 +5800,22 @@
       <c r="G129" t="s">
         <v>9</v>
       </c>
-      <c r="H129">
+      <c r="H129" s="4">
         <v>1573.0782099999999</v>
       </c>
-      <c r="I129">
+      <c r="I129" s="4">
         <v>420.18555241495221</v>
       </c>
-      <c r="J129">
+      <c r="J129" s="4">
         <v>4930.3203350000003</v>
       </c>
-      <c r="K129">
+      <c r="K129" s="4">
         <v>3531.2043232445271</v>
       </c>
-      <c r="L129">
+      <c r="L129" s="4">
         <v>6503.398545</v>
       </c>
-      <c r="M129">
+      <c r="M129" s="4">
         <v>3163.6514503128392</v>
       </c>
     </row>
@@ -5840,22 +5841,22 @@
       <c r="G130" t="s">
         <v>9</v>
       </c>
-      <c r="H130">
+      <c r="H130" s="4">
         <v>2103.1194800000003</v>
       </c>
-      <c r="I130">
+      <c r="I130" s="4">
         <v>1440.0025078239305</v>
       </c>
-      <c r="J130">
+      <c r="J130" s="4">
         <v>6884.4834824999998</v>
       </c>
-      <c r="K130">
+      <c r="K130" s="4">
         <v>4628.9935019772265</v>
       </c>
-      <c r="L130">
+      <c r="L130" s="4">
         <v>8987.602962500001</v>
       </c>
-      <c r="M130">
+      <c r="M130" s="4">
         <v>3200.9701871054681</v>
       </c>
     </row>
@@ -5881,22 +5882,22 @@
       <c r="G131" t="s">
         <v>9</v>
       </c>
-      <c r="H131">
+      <c r="H131" s="4">
         <v>2429.2987250000001</v>
       </c>
-      <c r="I131">
+      <c r="I131" s="4">
         <v>2087.6179902945128</v>
       </c>
-      <c r="J131">
+      <c r="J131" s="4">
         <v>7272.6779000000006</v>
       </c>
-      <c r="K131">
+      <c r="K131" s="4">
         <v>4910.4188932006327</v>
       </c>
-      <c r="L131">
+      <c r="L131" s="4">
         <v>9701.9766249999993</v>
       </c>
-      <c r="M131">
+      <c r="M131" s="4">
         <v>2873.885144618614</v>
       </c>
     </row>
@@ -5922,22 +5923,22 @@
       <c r="G132" t="s">
         <v>8</v>
       </c>
-      <c r="H132">
+      <c r="H132" s="4">
         <v>4967.6322250000003</v>
       </c>
-      <c r="I132">
+      <c r="I132" s="4">
         <v>3408.9085142597964</v>
       </c>
-      <c r="J132">
+      <c r="J132" s="4">
         <v>0</v>
       </c>
-      <c r="K132">
+      <c r="K132" s="4">
         <v>0</v>
       </c>
-      <c r="L132">
+      <c r="L132" s="4">
         <v>4967.6322250000003</v>
       </c>
-      <c r="M132">
+      <c r="M132" s="4">
         <v>3408.9085142597964</v>
       </c>
     </row>
@@ -5963,22 +5964,22 @@
       <c r="G133" t="s">
         <v>8</v>
       </c>
-      <c r="H133">
+      <c r="H133" s="4">
         <v>6133.7230225000003</v>
       </c>
-      <c r="I133">
+      <c r="I133" s="4">
         <v>1269.8428995291067</v>
       </c>
-      <c r="J133">
+      <c r="J133" s="4">
         <v>2026.7768624999999</v>
       </c>
-      <c r="K133">
+      <c r="K133" s="4">
         <v>1765.9053955556785</v>
       </c>
-      <c r="L133">
+      <c r="L133" s="4">
         <v>8160.4998849999993</v>
       </c>
-      <c r="M133">
+      <c r="M133" s="4">
         <v>2519.9093906419967</v>
       </c>
     </row>
@@ -6004,22 +6005,22 @@
       <c r="G134" t="s">
         <v>8</v>
       </c>
-      <c r="H134">
+      <c r="H134" s="4">
         <v>6821.4175950000008</v>
       </c>
-      <c r="I134">
+      <c r="I134" s="4">
         <v>1069.2829381508084</v>
       </c>
-      <c r="J134">
+      <c r="J134" s="4">
         <v>2430.423675</v>
       </c>
-      <c r="K134">
+      <c r="K134" s="4">
         <v>2059.3439645009994</v>
       </c>
-      <c r="L134">
+      <c r="L134" s="4">
         <v>9251.8412700000008</v>
       </c>
-      <c r="M134">
+      <c r="M134" s="4">
         <v>2079.5099186433436</v>
       </c>
     </row>
@@ -6045,22 +6046,22 @@
       <c r="G135" t="s">
         <v>8</v>
       </c>
-      <c r="H135">
+      <c r="H135" s="4">
         <v>7673.5608700000003</v>
       </c>
-      <c r="I135">
+      <c r="I135" s="4">
         <v>1346.1807603318744</v>
       </c>
-      <c r="J135">
+      <c r="J135" s="4">
         <v>3402.1660075</v>
       </c>
-      <c r="K135">
+      <c r="K135" s="4">
         <v>2948.4249959366243</v>
       </c>
-      <c r="L135">
+      <c r="L135" s="4">
         <v>11075.726877500001</v>
       </c>
-      <c r="M135">
+      <c r="M135" s="4">
         <v>2229.2343899938273</v>
       </c>
     </row>
@@ -6086,22 +6087,22 @@
       <c r="G136" t="s">
         <v>8</v>
       </c>
-      <c r="H136">
+      <c r="H136" s="4">
         <v>8413.5800275000001</v>
       </c>
-      <c r="I136">
+      <c r="I136" s="4">
         <v>1427.9768737046181</v>
       </c>
-      <c r="J136">
+      <c r="J136" s="4">
         <v>3626.4142375000001</v>
       </c>
-      <c r="K136">
+      <c r="K136" s="4">
         <v>3285.3404278613175</v>
       </c>
-      <c r="L136">
+      <c r="L136" s="4">
         <v>12039.994265000001</v>
       </c>
-      <c r="M136">
+      <c r="M136" s="4">
         <v>2505.9012694780267</v>
       </c>
     </row>
@@ -6127,22 +6128,22 @@
       <c r="G137" t="s">
         <v>9</v>
       </c>
-      <c r="H137">
+      <c r="H137" s="4">
         <v>1211.7272782499999</v>
       </c>
-      <c r="I137">
+      <c r="I137" s="4">
         <v>1551.2060889032214</v>
       </c>
-      <c r="J137">
+      <c r="J137" s="4">
         <v>0</v>
       </c>
-      <c r="K137">
+      <c r="K137" s="4">
         <v>0</v>
       </c>
-      <c r="L137">
+      <c r="L137" s="4">
         <v>1211.7272782499999</v>
       </c>
-      <c r="M137">
+      <c r="M137" s="4">
         <v>1551.2060889032214</v>
       </c>
     </row>
@@ -6168,22 +6169,22 @@
       <c r="G138" t="s">
         <v>9</v>
       </c>
-      <c r="H138">
+      <c r="H138" s="4">
         <v>1831.707678</v>
       </c>
-      <c r="I138">
+      <c r="I138" s="4">
         <v>1187.8684905963028</v>
       </c>
-      <c r="J138">
+      <c r="J138" s="4">
         <v>1505.4793452500001</v>
       </c>
-      <c r="K138">
+      <c r="K138" s="4">
         <v>1903.1768375043769</v>
       </c>
-      <c r="L138">
+      <c r="L138" s="4">
         <v>3337.1870232500005</v>
       </c>
-      <c r="M138">
+      <c r="M138" s="4">
         <v>2974.0964136771654</v>
       </c>
     </row>
@@ -6209,22 +6210,22 @@
       <c r="G139" t="s">
         <v>9</v>
       </c>
-      <c r="H139">
+      <c r="H139" s="4">
         <v>2680.333333</v>
       </c>
-      <c r="I139">
+      <c r="I139" s="4">
         <v>1359.1264525105432</v>
       </c>
-      <c r="J139">
+      <c r="J139" s="4">
         <v>4844.0549107500001</v>
       </c>
-      <c r="K139">
+      <c r="K139" s="4">
         <v>2834.7603881589594</v>
       </c>
-      <c r="L139">
+      <c r="L139" s="4">
         <v>7524.3882437499997</v>
       </c>
-      <c r="M139">
+      <c r="M139" s="4">
         <v>2925.2105001129203</v>
       </c>
     </row>
@@ -6250,22 +6251,22 @@
       <c r="G140" t="s">
         <v>9</v>
       </c>
-      <c r="H140">
+      <c r="H140" s="4">
         <v>3471.7976755</v>
       </c>
-      <c r="I140">
+      <c r="I140" s="4">
         <v>2458.8204517573763</v>
       </c>
-      <c r="J140">
+      <c r="J140" s="4">
         <v>5417.1337207500001</v>
       </c>
-      <c r="K140">
+      <c r="K140" s="4">
         <v>3189.2902025353005</v>
       </c>
-      <c r="L140">
+      <c r="L140" s="4">
         <v>8888.9313962499982</v>
       </c>
-      <c r="M140">
+      <c r="M140" s="4">
         <v>1694.1716766774507</v>
       </c>
     </row>
@@ -6291,22 +6292,22 @@
       <c r="G141" t="s">
         <v>9</v>
       </c>
-      <c r="H141">
+      <c r="H141" s="4">
         <v>3630.0905454999997</v>
       </c>
-      <c r="I141">
+      <c r="I141" s="4">
         <v>2736.2148785923528</v>
       </c>
-      <c r="J141">
+      <c r="J141" s="4">
         <v>5558.7641807500004</v>
       </c>
-      <c r="K141">
+      <c r="K141" s="4">
         <v>3303.9488692455288</v>
       </c>
-      <c r="L141">
+      <c r="L141" s="4">
         <v>9188.8547262499997</v>
       </c>
-      <c r="M141">
+      <c r="M141" s="4">
         <v>1399.8472055075172</v>
       </c>
     </row>
@@ -6332,22 +6333,22 @@
       <c r="G142" t="s">
         <v>8</v>
       </c>
-      <c r="H142">
+      <c r="H142" s="4">
         <v>1007.0342352499999</v>
       </c>
-      <c r="I142">
+      <c r="I142" s="4">
         <v>431.59270399161778</v>
       </c>
-      <c r="J142">
+      <c r="J142" s="4">
         <v>0</v>
       </c>
-      <c r="K142">
+      <c r="K142" s="4">
         <v>0</v>
       </c>
-      <c r="L142">
+      <c r="L142" s="4">
         <v>1007.0342352499999</v>
       </c>
-      <c r="M142">
+      <c r="M142" s="4">
         <v>431.59270399161778</v>
       </c>
     </row>
@@ -6373,22 +6374,22 @@
       <c r="G143" t="s">
         <v>8</v>
       </c>
-      <c r="H143">
+      <c r="H143" s="4">
         <v>1785.8728375000001</v>
       </c>
-      <c r="I143">
+      <c r="I143" s="4">
         <v>373.46374712909687</v>
       </c>
-      <c r="J143">
+      <c r="J143" s="4">
         <v>1843.5763400000001</v>
       </c>
-      <c r="K143">
+      <c r="K143" s="4">
         <v>2017.9986787737967</v>
       </c>
-      <c r="L143">
+      <c r="L143" s="4">
         <v>3629.4491775000001</v>
       </c>
-      <c r="M143">
+      <c r="M143" s="4">
         <v>1797.2496746621996</v>
       </c>
     </row>
@@ -6414,22 +6415,22 @@
       <c r="G144" t="s">
         <v>8</v>
       </c>
-      <c r="H144">
+      <c r="H144" s="4">
         <v>2706.6096874999998</v>
       </c>
-      <c r="I144">
+      <c r="I144" s="4">
         <v>1675.1110880918391</v>
       </c>
-      <c r="J144">
+      <c r="J144" s="4">
         <v>5225.9061450000008</v>
       </c>
-      <c r="K144">
+      <c r="K144" s="4">
         <v>3219.7109258448518</v>
       </c>
-      <c r="L144">
+      <c r="L144" s="4">
         <v>7932.5158324999993</v>
       </c>
-      <c r="M144">
+      <c r="M144" s="4">
         <v>1668.081377924932</v>
       </c>
     </row>
@@ -6455,22 +6456,22 @@
       <c r="G145" t="s">
         <v>8</v>
       </c>
-      <c r="H145">
+      <c r="H145" s="4">
         <v>3491.4784924999994</v>
       </c>
-      <c r="I145">
+      <c r="I145" s="4">
         <v>2430.9324575544028</v>
       </c>
-      <c r="J145">
+      <c r="J145" s="4">
         <v>5990.9883449999998</v>
       </c>
-      <c r="K145">
+      <c r="K145" s="4">
         <v>2316.4723282748819</v>
       </c>
-      <c r="L145">
+      <c r="L145" s="4">
         <v>9482.4668374999983</v>
       </c>
-      <c r="M145">
+      <c r="M145" s="4">
         <v>256.67351676682944</v>
       </c>
     </row>
@@ -6496,22 +6497,22 @@
       <c r="G146" t="s">
         <v>8</v>
       </c>
-      <c r="H146">
+      <c r="H146" s="4">
         <v>3715.7267224999996</v>
       </c>
-      <c r="I146">
+      <c r="I146" s="4">
         <v>2223.1132802521238</v>
       </c>
-      <c r="J146">
+      <c r="J146" s="4">
         <v>6659.9641599999995</v>
       </c>
-      <c r="K146">
+      <c r="K146" s="4">
         <v>2563.2797124173794</v>
       </c>
-      <c r="L146">
+      <c r="L146" s="4">
         <v>10375.690882499999</v>
       </c>
-      <c r="M146">
+      <c r="M146" s="4">
         <v>905.96694488106255</v>
       </c>
     </row>
@@ -6537,22 +6538,22 @@
       <c r="G147" t="s">
         <v>9</v>
       </c>
-      <c r="H147">
+      <c r="H147" s="4">
         <v>74.749409999999997</v>
       </c>
-      <c r="I147">
+      <c r="I147" s="4">
         <v>149.49881999999999</v>
       </c>
-      <c r="J147">
+      <c r="J147" s="4">
         <v>0</v>
       </c>
-      <c r="K147">
+      <c r="K147" s="4">
         <v>0</v>
       </c>
-      <c r="L147">
+      <c r="L147" s="4">
         <v>74.749409999999997</v>
       </c>
-      <c r="M147">
+      <c r="M147" s="4">
         <v>149.49881999999999</v>
       </c>
     </row>
@@ -6578,22 +6579,22 @@
       <c r="G148" t="s">
         <v>9</v>
       </c>
-      <c r="H148">
+      <c r="H148" s="4">
         <v>697.66116024999997</v>
       </c>
-      <c r="I148">
+      <c r="I148" s="4">
         <v>986.64187441294575</v>
       </c>
-      <c r="J148">
+      <c r="J148" s="4">
         <v>1017.045003</v>
       </c>
-      <c r="K148">
+      <c r="K148" s="4">
         <v>815.52780432582153</v>
       </c>
-      <c r="L148">
+      <c r="L148" s="4">
         <v>1714.7061632499999</v>
       </c>
-      <c r="M148">
+      <c r="M148" s="4">
         <v>1484.3315464537386</v>
       </c>
     </row>
@@ -6619,22 +6620,22 @@
       <c r="G149" t="s">
         <v>9</v>
       </c>
-      <c r="H149">
+      <c r="H149" s="4">
         <v>1575.6003090000002</v>
       </c>
-      <c r="I149">
+      <c r="I149" s="4">
         <v>1928.530151439664</v>
       </c>
-      <c r="J149">
+      <c r="J149" s="4">
         <v>2407.8370574999999</v>
       </c>
-      <c r="K149">
+      <c r="K149" s="4">
         <v>2225.5788152383439</v>
       </c>
-      <c r="L149">
+      <c r="L149" s="4">
         <v>3983.4373665000003</v>
       </c>
-      <c r="M149">
+      <c r="M149" s="4">
         <v>3290.3769966654277</v>
       </c>
     </row>
@@ -6660,22 +6661,22 @@
       <c r="G150" t="s">
         <v>9</v>
       </c>
-      <c r="H150">
+      <c r="H150" s="4">
         <v>2748.1400775000002</v>
       </c>
-      <c r="I150">
+      <c r="I150" s="4">
         <v>2392.6773385604474</v>
       </c>
-      <c r="J150">
+      <c r="J150" s="4">
         <v>4011.5516725000002</v>
       </c>
-      <c r="K150">
+      <c r="K150" s="4">
         <v>3389.0063230586375</v>
       </c>
-      <c r="L150">
+      <c r="L150" s="4">
         <v>6759.69175</v>
       </c>
-      <c r="M150">
+      <c r="M150" s="4">
         <v>3368.5885942949094</v>
       </c>
     </row>
@@ -6701,22 +6702,22 @@
       <c r="G151" t="s">
         <v>9</v>
       </c>
-      <c r="H151">
+      <c r="H151" s="4">
         <v>4379.0362949999999</v>
       </c>
-      <c r="I151">
+      <c r="I151" s="4">
         <v>3491.0047994887691</v>
       </c>
-      <c r="J151">
+      <c r="J151" s="4">
         <v>5719.4624299999996</v>
       </c>
-      <c r="K151">
+      <c r="K151" s="4">
         <v>4689.456877564462</v>
       </c>
-      <c r="L151">
+      <c r="L151" s="4">
         <v>10098.498725000001</v>
       </c>
-      <c r="M151">
+      <c r="M151" s="4">
         <v>2154.9891083109828</v>
       </c>
     </row>
@@ -6742,22 +6743,22 @@
       <c r="G152" t="s">
         <v>8</v>
       </c>
-      <c r="H152">
+      <c r="H152" s="4">
         <v>2808.2905949999999</v>
       </c>
-      <c r="I152">
+      <c r="I152" s="4">
         <v>1329.9861969716237</v>
       </c>
-      <c r="J152">
+      <c r="J152" s="4">
         <v>0</v>
       </c>
-      <c r="K152">
+      <c r="K152" s="4">
         <v>0</v>
       </c>
-      <c r="L152">
+      <c r="L152" s="4">
         <v>2808.2905949999999</v>
       </c>
-      <c r="M152">
+      <c r="M152" s="4">
         <v>1329.9861969716237</v>
       </c>
     </row>
@@ -6783,22 +6784,22 @@
       <c r="G153" t="s">
         <v>8</v>
       </c>
-      <c r="H153">
+      <c r="H153" s="4">
         <v>4689.4840850000001</v>
       </c>
-      <c r="I153">
+      <c r="I153" s="4">
         <v>2346.3018974590555</v>
       </c>
-      <c r="J153">
+      <c r="J153" s="4">
         <v>1628.750305</v>
       </c>
-      <c r="K153">
+      <c r="K153" s="4">
         <v>3257.5006100000001</v>
       </c>
-      <c r="L153">
+      <c r="L153" s="4">
         <v>6318.2343899999996</v>
       </c>
-      <c r="M153">
+      <c r="M153" s="4">
         <v>1649.2812220352475</v>
       </c>
     </row>
@@ -6824,22 +6825,22 @@
       <c r="G154" t="s">
         <v>8</v>
       </c>
-      <c r="H154">
+      <c r="H154" s="4">
         <v>6344.3851100000002</v>
       </c>
-      <c r="I154">
+      <c r="I154" s="4">
         <v>1978.9866351981625</v>
       </c>
-      <c r="J154">
+      <c r="J154" s="4">
         <v>2550.9875427500001</v>
       </c>
-      <c r="K154">
+      <c r="K154" s="4">
         <v>3581.7328885648471</v>
       </c>
-      <c r="L154">
+      <c r="L154" s="4">
         <v>8895.3726527500003</v>
       </c>
-      <c r="M154">
+      <c r="M154" s="4">
         <v>1845.2964161173213</v>
       </c>
     </row>
@@ -6865,22 +6866,22 @@
       <c r="G155" t="s">
         <v>8</v>
       </c>
-      <c r="H155">
+      <c r="H155" s="4">
         <v>7620.9877775000004</v>
       </c>
-      <c r="I155">
+      <c r="I155" s="4">
         <v>3202.5959387536373</v>
       </c>
-      <c r="J155">
+      <c r="J155" s="4">
         <v>2739.8281577500002</v>
       </c>
-      <c r="K155">
+      <c r="K155" s="4">
         <v>3953.8967525035087</v>
       </c>
-      <c r="L155">
+      <c r="L155" s="4">
         <v>10360.815935250001</v>
       </c>
-      <c r="M155">
+      <c r="M155" s="4">
         <v>1823.0346562908701</v>
       </c>
     </row>
@@ -6906,22 +6907,22 @@
       <c r="G156" t="s">
         <v>8</v>
       </c>
-      <c r="H156">
+      <c r="H156" s="4">
         <v>7920.911105000001</v>
       </c>
-      <c r="I156">
+      <c r="I156" s="4">
         <v>3071.2207911431465</v>
       </c>
-      <c r="J156">
+      <c r="J156" s="4">
         <v>3597.2478609999998</v>
       </c>
-      <c r="K156">
+      <c r="K156" s="4">
         <v>3714.8830766766532</v>
       </c>
-      <c r="L156">
+      <c r="L156" s="4">
         <v>11518.158965999999</v>
       </c>
-      <c r="M156">
+      <c r="M156" s="4">
         <v>928.30429587998594</v>
       </c>
     </row>
@@ -6947,22 +6948,22 @@
       <c r="G157" t="s">
         <v>9</v>
       </c>
-      <c r="H157">
+      <c r="H157" s="4">
         <v>723.12726025000006</v>
       </c>
-      <c r="I157">
+      <c r="I157" s="4">
         <v>584.62522031212541</v>
       </c>
-      <c r="J157">
+      <c r="J157" s="4">
         <v>0</v>
       </c>
-      <c r="K157">
+      <c r="K157" s="4">
         <v>0</v>
       </c>
-      <c r="L157">
+      <c r="L157" s="4">
         <v>723.12726025000006</v>
       </c>
-      <c r="M157">
+      <c r="M157" s="4">
         <v>584.62522031212541</v>
       </c>
     </row>
@@ -6988,22 +6989,22 @@
       <c r="G158" t="s">
         <v>9</v>
       </c>
-      <c r="H158">
+      <c r="H158" s="4">
         <v>2621.1760049999998</v>
       </c>
-      <c r="I158">
+      <c r="I158" s="4">
         <v>1351.7403486716278</v>
       </c>
-      <c r="J158">
+      <c r="J158" s="4">
         <v>1472.45345275</v>
       </c>
-      <c r="K158">
+      <c r="K158" s="4">
         <v>1394.2176732666831</v>
       </c>
-      <c r="L158">
+      <c r="L158" s="4">
         <v>4093.6294577500003</v>
       </c>
-      <c r="M158">
+      <c r="M158" s="4">
         <v>373.20349656797401</v>
       </c>
     </row>
@@ -7029,22 +7030,22 @@
       <c r="G159" t="s">
         <v>9</v>
       </c>
-      <c r="H159">
+      <c r="H159" s="4">
         <v>3899.7939774999995</v>
       </c>
-      <c r="I159">
+      <c r="I159" s="4">
         <v>1668.1015408004464</v>
       </c>
-      <c r="J159">
+      <c r="J159" s="4">
         <v>4233.7846024999999</v>
       </c>
-      <c r="K159">
+      <c r="K159" s="4">
         <v>3416.8006159724337</v>
       </c>
-      <c r="L159">
+      <c r="L159" s="4">
         <v>8133.5785800000003</v>
       </c>
-      <c r="M159">
+      <c r="M159" s="4">
         <v>1928.7103503917021</v>
       </c>
     </row>
@@ -7070,22 +7071,22 @@
       <c r="G160" t="s">
         <v>9</v>
       </c>
-      <c r="H160">
+      <c r="H160" s="4">
         <v>5114.838310000001</v>
       </c>
-      <c r="I160">
+      <c r="I160" s="4">
         <v>3185.2251868886892</v>
       </c>
-      <c r="J160">
+      <c r="J160" s="4">
         <v>4626.2190049999999</v>
       </c>
-      <c r="K160">
+      <c r="K160" s="4">
         <v>3875.2392768046811</v>
       </c>
-      <c r="L160">
+      <c r="L160" s="4">
         <v>9741.057315</v>
       </c>
-      <c r="M160">
+      <c r="M160" s="4">
         <v>1387.7708455987683</v>
       </c>
     </row>
@@ -7111,22 +7112,22 @@
       <c r="G161" t="s">
         <v>9</v>
       </c>
-      <c r="H161">
+      <c r="H161" s="4">
         <v>6036.7477024999998</v>
       </c>
-      <c r="I161">
+      <c r="I161" s="4">
         <v>2589.5363805256784</v>
       </c>
-      <c r="J161">
+      <c r="J161" s="4">
         <v>5064.8221599999997</v>
       </c>
-      <c r="K161">
+      <c r="K161" s="4">
         <v>4143.5148198013858</v>
       </c>
-      <c r="L161">
+      <c r="L161" s="4">
         <v>11101.5698625</v>
       </c>
-      <c r="M161">
+      <c r="M161" s="4">
         <v>1790.0290413136777</v>
       </c>
     </row>
@@ -9080,10 +9081,10 @@
         <v>9</v>
       </c>
       <c r="H209" s="4">
-        <v>68136.75</v>
+        <v>32618.42</v>
       </c>
       <c r="I209" s="4">
-        <v>69449.628476928032</v>
+        <v>3478.9642729218513</v>
       </c>
       <c r="J209" s="4">
         <v>9088.75</v>
@@ -9092,10 +9093,10 @@
         <v>1727.5285574098816</v>
       </c>
       <c r="L209" s="4">
-        <v>77225.5</v>
+        <v>41707.17</v>
       </c>
       <c r="M209" s="4">
-        <v>70933.321020518983</v>
+        <v>2273.9672195526477</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.2">
@@ -9121,10 +9122,10 @@
         <v>9</v>
       </c>
       <c r="H210" s="4">
-        <v>82666.75</v>
+        <v>47148.639999999999</v>
       </c>
       <c r="I210" s="4">
-        <v>70287.392147643855</v>
+        <v>3209.5266294372241</v>
       </c>
       <c r="J210" s="4">
         <v>12646.5</v>
@@ -9133,10 +9134,10 @@
         <v>1680.9740231980584</v>
       </c>
       <c r="L210" s="4">
-        <v>95313.25</v>
+        <v>59795.14</v>
       </c>
       <c r="M210" s="4">
-        <v>71550.955904981922</v>
+        <v>2333.3093290574798</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.2">
@@ -9162,10 +9163,10 @@
         <v>9</v>
       </c>
       <c r="H211" s="4">
-        <v>107481.5</v>
+        <v>71963.385000000009</v>
       </c>
       <c r="I211" s="4">
-        <v>79901.689254149489</v>
+        <v>12542.237427438225</v>
       </c>
       <c r="J211" s="4">
         <v>19822</v>
@@ -9174,10 +9175,10 @@
         <v>1308.0129968773247</v>
       </c>
       <c r="L211" s="4">
-        <v>127303.5</v>
+        <v>91785.385000000009</v>
       </c>
       <c r="M211" s="4">
-        <v>79904.486655422967</v>
+        <v>13324.796100237276</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>